<commit_message>
Purhcaseorder updated for multi user
</commit_message>
<xml_diff>
--- a/Migration_Status_Overall.xlsx
+++ b/Migration_Status_Overall.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dixitp\OneDrive - International Shared Support Centre\Dixit_Work\Hawaii_Forest_Trail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://isscindia-my.sharepoint.com/personal/dixitp_issc_co_in/Documents/Dixit_Work/Hawaii_Forest_Trail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E6D411-BE56-4C72-BA10-F07CC969BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{B9E6D411-BE56-4C72-BA10-F07CC969BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E24C78AA-1021-4727-A3DE-FD3598ADAE64}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hawaii Forest &amp; Trail (IES)" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hawaii Forest &amp; Trail (IES)'!$B$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="345">
   <si>
     <t>Table Name</t>
   </si>
@@ -1086,12 +1087,15 @@
   <si>
     <t>Can not migrate no location level filter present. Migrated where account ref name like kozi</t>
   </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,8 +1133,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1155,6 +1165,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1169,7 +1185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1178,6 +1194,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1194,6 +1215,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1459,15 +1484,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
@@ -2133,34 +2160,340 @@
     <row r="25" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
       <c r="B25" s="4"/>
     </row>
-    <row r="26" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B32" s="4"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>D27-E27-G27</f>
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F39" si="3">D28-E28-G28</f>
+        <v>25</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="10">
+        <v>25</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="G31" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>44</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="11">
+        <v>8</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11">
+        <v>68</v>
+      </c>
+      <c r="E34" s="11">
+        <v>0</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="G34" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>20</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>11</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>33</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>21</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{99AA452C-C8B1-45EA-A340-4449531578F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C25 C27:C1048576" xr:uid="{99AA452C-C8B1-45EA-A340-4449531578F0}">
       <formula1>"Completed, Pending, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7973,15 +8306,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2435A5-9F5A-4EB8-AF54-E1E6DDA13E40}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
@@ -8589,9 +8923,326 @@
         <v>49</v>
       </c>
     </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f>D28-E28-G28</f>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:F40" si="1">D29-E29-G29</f>
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>67</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>11</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C24" xr:uid="{81987673-4498-4E3B-B774-63A09DEE5898}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C24 C28:C40" xr:uid="{81987673-4498-4E3B-B774-63A09DEE5898}">
       <formula1>"Completed, Pending, NA"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>